<commit_message>
done xuat file error và success full
</commit_message>
<xml_diff>
--- a/source-code/net-core/host/Ord.Zero.HttpHost/Contents/Excel/MasterData/ListCountry_vi.xlsx
+++ b/source-code/net-core/host/Ord.Zero.HttpHost/Contents/Excel/MasterData/ListCountry_vi.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A51560-6173-4251-A9B1-90949BE8209B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E8E043-1A16-40B8-8641-E5E01C0C6CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -151,7 +164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -161,6 +174,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -471,11 +490,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -486,10 +505,11 @@
     <col min="4" max="4" width="32.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="29.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="28.42578125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="85.28515625" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -508,6 +528,7 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="5"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>